<commit_message>
fin of... accountFolder n tripFolder_new,delet,edit
</commit_message>
<xml_diff>
--- a/doc/詳細設計/trip_詳細設計_メニュー.xlsx
+++ b/doc/詳細設計/trip_詳細設計_メニュー.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="555" yWindow="1320" windowWidth="13110" windowHeight="8745" tabRatio="908" activeTab="1"/>
+    <workbookView xWindow="555" yWindow="1320" windowWidth="13110" windowHeight="8745" tabRatio="908"/>
   </bookViews>
   <sheets>
     <sheet name="trip" sheetId="13" r:id="rId1"/>
@@ -499,6 +499,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -508,38 +532,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -823,7 +823,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="U43" sqref="U43"/>
     </sheetView>
   </sheetViews>
@@ -874,38 +874,38 @@
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B3" s="9"/>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
-      <c r="J3" s="31" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
+      <c r="J3" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="33"/>
-      <c r="O3" s="31" t="s">
+      <c r="K3" s="28"/>
+      <c r="L3" s="29"/>
+      <c r="O3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="31" t="s">
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="U3" s="33"/>
+      <c r="U3" s="29"/>
       <c r="V3" s="8"/>
       <c r="W3" s="8"/>
-      <c r="X3" s="31" t="s">
+      <c r="X3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Y3" s="32"/>
-      <c r="Z3" s="32"/>
-      <c r="AA3" s="33"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="29"/>
       <c r="AB3" s="12"/>
     </row>
     <row r="4" spans="2:28" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -939,41 +939,41 @@
     </row>
     <row r="5" spans="2:28" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B5" s="17"/>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="30"/>
-      <c r="J5" s="34" t="s">
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="34"/>
-      <c r="L5" s="34"/>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34" t="s">
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34" t="s">
+      <c r="O5" s="30"/>
+      <c r="P5" s="30"/>
+      <c r="Q5" s="30"/>
+      <c r="R5" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="28" t="s">
+      <c r="S5" s="30"/>
+      <c r="T5" s="30"/>
+      <c r="U5" s="30"/>
+      <c r="V5" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="30"/>
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="26"/>
       <c r="AB5" s="18"/>
     </row>
     <row r="6" spans="2:28" ht="6" customHeight="1" x14ac:dyDescent="0.15">
@@ -1007,142 +1007,142 @@
     </row>
     <row r="7" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B7" s="9"/>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27" t="s">
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27" t="s">
+      <c r="K7" s="31"/>
+      <c r="L7" s="31"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27" t="s">
+      <c r="O7" s="31"/>
+      <c r="P7" s="31"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="27"/>
-      <c r="V7" s="27" t="s">
+      <c r="S7" s="31"/>
+      <c r="T7" s="31"/>
+      <c r="U7" s="31"/>
+      <c r="V7" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="W7" s="27"/>
-      <c r="X7" s="27" t="s">
+      <c r="W7" s="31"/>
+      <c r="X7" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Y7" s="27"/>
-      <c r="Z7" s="24" t="s">
+      <c r="Y7" s="31"/>
+      <c r="Z7" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="AA7" s="24"/>
+      <c r="AA7" s="32"/>
       <c r="AB7" s="12"/>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B8" s="9"/>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27" t="s">
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27" t="s">
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27" t="s">
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="27" t="s">
+      <c r="S8" s="31"/>
+      <c r="T8" s="31"/>
+      <c r="U8" s="31"/>
+      <c r="V8" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="W8" s="27"/>
-      <c r="X8" s="27" t="s">
+      <c r="W8" s="31"/>
+      <c r="X8" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Y8" s="27"/>
-      <c r="Z8" s="24" t="s">
+      <c r="Y8" s="31"/>
+      <c r="Z8" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="AA8" s="24"/>
+      <c r="AA8" s="32"/>
       <c r="AB8" s="12"/>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B9" s="9"/>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27" t="s">
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27" t="s">
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27" t="s">
+      <c r="O9" s="31"/>
+      <c r="P9" s="31"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="27" t="s">
+      <c r="S9" s="31"/>
+      <c r="T9" s="31"/>
+      <c r="U9" s="31"/>
+      <c r="V9" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="W9" s="27"/>
-      <c r="X9" s="27" t="s">
+      <c r="W9" s="31"/>
+      <c r="X9" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="24" t="s">
+      <c r="Y9" s="31"/>
+      <c r="Z9" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="AA9" s="24"/>
+      <c r="AA9" s="32"/>
       <c r="AB9" s="12"/>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B10" s="9"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -1165,13 +1165,13 @@
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B11" s="9"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -1194,13 +1194,13 @@
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B12" s="9"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
@@ -1223,13 +1223,13 @@
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B13" s="9"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
       <c r="J13" s="6"/>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -1252,13 +1252,13 @@
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B14" s="9"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
       <c r="J14" s="6"/>
       <c r="K14" s="6"/>
       <c r="L14" s="6"/>
@@ -1281,13 +1281,13 @@
     </row>
     <row r="15" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B15" s="9"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
       <c r="J15" s="6"/>
       <c r="K15" s="6"/>
       <c r="L15" s="6"/>
@@ -1310,13 +1310,13 @@
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B16" s="9"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
       <c r="J16" s="6"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
@@ -1339,13 +1339,13 @@
     </row>
     <row r="17" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B17" s="9"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
       <c r="J17" s="6"/>
       <c r="K17" s="6"/>
       <c r="L17" s="6"/>
@@ -1368,13 +1368,13 @@
     </row>
     <row r="18" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B18" s="9"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
@@ -1397,13 +1397,13 @@
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B19" s="9"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
@@ -1426,13 +1426,13 @@
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B20" s="9"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6"/>
       <c r="L20" s="6"/>
@@ -1455,13 +1455,13 @@
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B21" s="9"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
-      <c r="G21" s="24"/>
-      <c r="H21" s="24"/>
-      <c r="I21" s="24"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
       <c r="L21" s="6"/>
@@ -1484,13 +1484,13 @@
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B22" s="9"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
       <c r="J22" s="6"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
@@ -1513,13 +1513,13 @@
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B23" s="9"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
       <c r="L23" s="6"/>
@@ -1542,13 +1542,13 @@
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B24" s="7"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="34"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
@@ -1571,13 +1571,13 @@
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B25" s="7"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="34"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="6"/>
@@ -1600,13 +1600,13 @@
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B26" s="7"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="34"/>
+      <c r="I26" s="34"/>
       <c r="J26" s="6"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
@@ -1629,13 +1629,13 @@
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B27" s="7"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
@@ -1658,13 +1658,13 @@
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B28" s="7"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="34"/>
       <c r="J28" s="6"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
@@ -1687,13 +1687,13 @@
     </row>
     <row r="29" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B29" s="7"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="34"/>
       <c r="J29" s="6"/>
       <c r="K29" s="6"/>
       <c r="L29" s="6"/>
@@ -1716,13 +1716,13 @@
     </row>
     <row r="30" spans="2:28" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
@@ -1745,23 +1745,25 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="V5:AA5"/>
-    <mergeCell ref="X3:AA3"/>
-    <mergeCell ref="O3:S3"/>
-    <mergeCell ref="T3:U3"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="R5:U5"/>
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="V8:W8"/>
-    <mergeCell ref="X8:Y8"/>
-    <mergeCell ref="Z8:AA8"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="N7:Q7"/>
-    <mergeCell ref="R7:U7"/>
-    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C14:I14"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="C17:I17"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="C19:I19"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="C28:I28"/>
+    <mergeCell ref="C29:I29"/>
     <mergeCell ref="Z9:AA9"/>
     <mergeCell ref="C11:I11"/>
     <mergeCell ref="C7:I7"/>
@@ -1778,25 +1780,23 @@
     <mergeCell ref="J8:M8"/>
     <mergeCell ref="N8:Q8"/>
     <mergeCell ref="R8:U8"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="C28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="C13:I13"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="C15:I15"/>
-    <mergeCell ref="C16:I16"/>
-    <mergeCell ref="C17:I17"/>
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="C19:I19"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="V8:W8"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="R7:U7"/>
+    <mergeCell ref="V7:W7"/>
+    <mergeCell ref="V5:AA5"/>
+    <mergeCell ref="X3:AA3"/>
+    <mergeCell ref="O3:S3"/>
+    <mergeCell ref="T3:U3"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="R5:U5"/>
+    <mergeCell ref="J3:L3"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1808,7 +1808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -1859,38 +1859,38 @@
     </row>
     <row r="3" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B3" s="9"/>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="33"/>
-      <c r="J3" s="31" t="s">
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="29"/>
+      <c r="J3" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="33"/>
-      <c r="O3" s="31" t="s">
+      <c r="K3" s="28"/>
+      <c r="L3" s="29"/>
+      <c r="O3" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="32"/>
-      <c r="Q3" s="32"/>
-      <c r="R3" s="32"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="31" t="s">
+      <c r="P3" s="28"/>
+      <c r="Q3" s="28"/>
+      <c r="R3" s="28"/>
+      <c r="S3" s="29"/>
+      <c r="T3" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="U3" s="33"/>
+      <c r="U3" s="29"/>
       <c r="V3" s="20"/>
       <c r="W3" s="20"/>
-      <c r="X3" s="31" t="s">
+      <c r="X3" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="Y3" s="32"/>
-      <c r="Z3" s="32"/>
-      <c r="AA3" s="33"/>
+      <c r="Y3" s="28"/>
+      <c r="Z3" s="28"/>
+      <c r="AA3" s="29"/>
       <c r="AB3" s="12"/>
     </row>
     <row r="4" spans="2:28" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -1969,10 +1969,10 @@
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B8" s="9"/>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="35"/>
+      <c r="D8" s="37"/>
       <c r="E8" s="36"/>
       <c r="F8" s="36"/>
       <c r="G8" s="36"/>
@@ -2066,15 +2066,15 @@
     </row>
     <row r="16" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B16" s="9"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="37"/>
-      <c r="K16" s="37"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
+      <c r="G16" s="35"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="35"/>
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>
@@ -2085,15 +2085,15 @@
     </row>
     <row r="17" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B17" s="9"/>
-      <c r="C17" s="37"/>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
+      <c r="G17" s="35"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="35"/>
       <c r="L17" s="21"/>
       <c r="M17" s="21"/>
       <c r="N17" s="21"/>
@@ -2104,15 +2104,15 @@
     </row>
     <row r="18" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B18" s="9"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="35"/>
+      <c r="F18" s="35"/>
+      <c r="G18" s="35"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="35"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18" s="21"/>
@@ -2123,15 +2123,15 @@
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B19" s="9"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="35"/>
       <c r="L19" s="21"/>
       <c r="M19" s="21"/>
       <c r="N19" s="21"/>
@@ -2142,15 +2142,15 @@
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B20" s="9"/>
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
       <c r="L20" s="21"/>
       <c r="M20" s="21"/>
       <c r="N20" s="21"/>
@@ -2160,15 +2160,15 @@
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B21" s="9"/>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
       <c r="L21" s="21"/>
       <c r="M21" s="21"/>
       <c r="N21" s="21"/>
@@ -2179,15 +2179,15 @@
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B22" s="9"/>
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
       <c r="L22" s="21"/>
       <c r="M22" s="21"/>
       <c r="N22" s="21"/>
@@ -2197,15 +2197,15 @@
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B23" s="9"/>
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35"/>
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
       <c r="N23" s="21"/>
@@ -2216,15 +2216,15 @@
     </row>
     <row r="24" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B24" s="9"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="35"/>
       <c r="L24" s="21"/>
       <c r="M24" s="21"/>
       <c r="N24" s="21"/>
@@ -2235,15 +2235,15 @@
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B25" s="9"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="35"/>
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
       <c r="N25" s="21"/>
@@ -2254,15 +2254,15 @@
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B26" s="9"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
       <c r="L26" s="21"/>
       <c r="M26" s="21"/>
       <c r="N26" s="21"/>
@@ -2331,15 +2331,15 @@
     </row>
     <row r="30" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B30" s="7"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="37"/>
-      <c r="E30" s="37"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
-      <c r="H30" s="37"/>
-      <c r="I30" s="37"/>
-      <c r="J30" s="37"/>
-      <c r="K30" s="37"/>
+      <c r="C30" s="35"/>
+      <c r="D30" s="35"/>
+      <c r="E30" s="35"/>
+      <c r="F30" s="35"/>
+      <c r="G30" s="35"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="35"/>
       <c r="L30" s="21"/>
       <c r="M30" s="21"/>
       <c r="N30" s="21"/>
@@ -2350,15 +2350,15 @@
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B31" s="7"/>
-      <c r="C31" s="37"/>
-      <c r="D31" s="37"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="37"/>
-      <c r="G31" s="37"/>
-      <c r="H31" s="37"/>
-      <c r="I31" s="37"/>
-      <c r="J31" s="37"/>
-      <c r="K31" s="37"/>
+      <c r="C31" s="35"/>
+      <c r="D31" s="35"/>
+      <c r="E31" s="35"/>
+      <c r="F31" s="35"/>
+      <c r="G31" s="35"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="35"/>
       <c r="L31" s="21"/>
       <c r="M31" s="21"/>
       <c r="N31" s="21"/>
@@ -2369,15 +2369,15 @@
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B32" s="7"/>
-      <c r="C32" s="37"/>
-      <c r="D32" s="37"/>
-      <c r="E32" s="37"/>
-      <c r="F32" s="37"/>
-      <c r="G32" s="37"/>
-      <c r="H32" s="37"/>
-      <c r="I32" s="37"/>
-      <c r="J32" s="37"/>
-      <c r="K32" s="37"/>
+      <c r="C32" s="35"/>
+      <c r="D32" s="35"/>
+      <c r="E32" s="35"/>
+      <c r="F32" s="35"/>
+      <c r="G32" s="35"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="35"/>
       <c r="L32" s="21"/>
       <c r="M32" s="21"/>
       <c r="N32" s="21"/>
@@ -2388,15 +2388,15 @@
     </row>
     <row r="33" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B33" s="7"/>
-      <c r="C33" s="37"/>
-      <c r="D33" s="37"/>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
+      <c r="C33" s="35"/>
+      <c r="D33" s="35"/>
+      <c r="E33" s="35"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="35"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="35"/>
       <c r="L33" s="21"/>
       <c r="M33" s="21"/>
       <c r="N33" s="21"/>
@@ -2407,15 +2407,15 @@
     </row>
     <row r="34" spans="2:28" x14ac:dyDescent="0.15">
       <c r="B34" s="7"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="37"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="37"/>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37"/>
-      <c r="I34" s="37"/>
-      <c r="J34" s="37"/>
-      <c r="K34" s="37"/>
+      <c r="C34" s="35"/>
+      <c r="D34" s="35"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="35"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="35"/>
       <c r="L34" s="21"/>
       <c r="M34" s="21"/>
       <c r="N34" s="21"/>
@@ -2474,6 +2474,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="X3:AA3"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="T3:U3"/>
     <mergeCell ref="C30:K34"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="O3:S3"/>
@@ -2485,12 +2491,6 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="C16:K26"/>
-    <mergeCell ref="X3:AA3"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="T3:U3"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="1">

</xml_diff>